<commit_message>
Comprobante de Pago y Nomina Lista
</commit_message>
<xml_diff>
--- a/HenriPittier/PlantillasExcel/NominaPlantilla.xlsx
+++ b/HenriPittier/PlantillasExcel/NominaPlantilla.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPGrock\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisAlejandro\Documents\GitHub\HPPasantia\HenriPittier\PlantillasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8232"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -128,13 +128,13 @@
     <t>COLEGIO</t>
   </si>
   <si>
-    <t>Estatus</t>
-  </si>
-  <si>
     <t>U.E. HENRI PITTIER FBS C.A.</t>
   </si>
   <si>
     <t xml:space="preserve"> J-31139418-4</t>
+  </si>
+  <si>
+    <t>TOTAL SUELDOS MENSUALES</t>
   </si>
 </sst>
 </file>
@@ -222,18 +222,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -254,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -560,60 +554,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,151 +566,137 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="10" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,6 +872,7 @@
       <sheetName val="descuentos esp"/>
       <sheetName val="Nomina Archivo"/>
       <sheetName val="formulas"/>
+      <sheetName val="nomina 1era de julio 2018"/>
     </sheetNames>
     <definedNames>
       <definedName name="iMPRIMIR_nOMINA"/>
@@ -957,6 +889,7 @@
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
+      <sheetData sheetId="11" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1228,18 +1161,18 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.20703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83984375" customWidth="1"/>
-    <col min="14" max="14" width="14.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1254,9 +1187,9 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="23.1" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1"/>
@@ -1273,19 +1206,19 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="6"/>
@@ -1302,7 +1235,7 @@
       <c r="T3" s="9"/>
       <c r="U3" s="9"/>
     </row>
-    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1325,7 +1258,7 @@
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
     </row>
-    <row r="5" spans="1:22" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1268,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -1350,7 +1283,7 @@
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
     </row>
-    <row r="6" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1373,11 +1306,11 @@
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
     </row>
-    <row r="7" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="57" t="s">
+    <row r="7" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1386,29 +1319,29 @@
       <c r="D7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="52" t="s">
+      <c r="J7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="53"/>
+      <c r="M7" s="50"/>
       <c r="N7" s="15" t="s">
         <v>14</v>
       </c>
@@ -1418,37 +1351,35 @@
       <c r="P7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="54" t="s">
+      <c r="Q7" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="54" t="s">
+      <c r="R7" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="S7" s="36" t="s">
+      <c r="S7" s="30" t="s">
         <v>19</v>
       </c>
       <c r="T7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="V7" s="30"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="58"/>
-      <c r="B8" s="40"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="51"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="16" t="s">
         <v>22</v>
       </c>
@@ -1470,22 +1401,22 @@
       <c r="P8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="37"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="31"/>
       <c r="T8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="U8" s="31"/>
-      <c r="V8" s="32"/>
-    </row>
-    <row r="9" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="59"/>
-      <c r="B9" s="41"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -1512,16 +1443,16 @@
       <c r="P9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="38"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="32"/>
       <c r="T9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="U9" s="33"/>
-      <c r="V9" s="34"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1545,7 +1476,7 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1569,7 +1500,7 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1593,7 +1524,7 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1617,7 +1548,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1641,7 +1572,7 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1665,7 +1596,7 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1689,7 +1620,7 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1713,7 +1644,7 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1737,7 +1668,7 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1761,7 +1692,7 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1785,7 +1716,7 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1809,7 +1740,7 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1833,7 +1764,7 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1857,7 +1788,7 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1881,7 +1812,7 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1905,7 +1836,7 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1929,7 +1860,7 @@
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1953,7 +1884,7 @@
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1977,7 +1908,7 @@
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -2001,7 +1932,7 @@
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -2025,7 +1956,7 @@
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -2049,7 +1980,7 @@
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -2073,10 +2004,15 @@
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="54"/>
+      <c r="C33" s="55">
+        <f>SUM(C10:C32)</f>
+        <v>0</v>
+      </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -2097,7 +2033,7 @@
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -2121,7 +2057,7 @@
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -2145,7 +2081,7 @@
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -2169,7 +2105,7 @@
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -2193,7 +2129,7 @@
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -2217,7 +2153,7 @@
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -2241,7 +2177,7 @@
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -2265,7 +2201,7 @@
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -2289,7 +2225,7 @@
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2313,7 +2249,7 @@
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2337,7 +2273,7 @@
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -2361,7 +2297,7 @@
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2385,7 +2321,7 @@
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -2409,7 +2345,7 @@
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -2433,7 +2369,7 @@
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -2457,7 +2393,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -2481,7 +2417,7 @@
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -2505,7 +2441,7 @@
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -2529,7 +2465,7 @@
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -2553,7 +2489,7 @@
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -2577,7 +2513,7 @@
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -2601,7 +2537,7 @@
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -2626,7 +2562,8 @@
       <c r="V55" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="S7:S9"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>

</xml_diff>